<commit_message>
Messung in der Konsole. Kleinere Umstellungen.
</commit_message>
<xml_diff>
--- a/bean-mapper-test/docs/jdk11-02/PerformanceTestWithCompleteFixtures.xlsx
+++ b/bean-mapper-test/docs/jdk11-02/PerformanceTestWithCompleteFixtures.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
-  <si>
-    <t>02.01.2022 um 20:20 Uhr</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+  <si>
+    <t>05.01.2022 um 17:56 Uhr</t>
   </si>
   <si>
     <t>Name des Messpunkts</t>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>JMapper</t>
+  </si>
+  <si>
+    <t>Selma</t>
   </si>
   <si>
     <t>reMap</t>
@@ -119,7 +122,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="1.0" ySplit="2.0" state="frozen" topLeftCell="B3" activePane="bottomRight"/>
@@ -167,7 +170,7 @@
         <v>10.0</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
@@ -176,10 +179,10 @@
         <v>2.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>0.632456</v>
+        <v>0.707107</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -193,19 +196,19 @@
         <v>10.0</v>
       </c>
       <c r="C4" t="n">
-        <v>210.0</v>
+        <v>188.0</v>
       </c>
       <c r="D4" t="n">
         <v>6.0</v>
       </c>
       <c r="E4" t="n">
-        <v>109.0</v>
+        <v>92.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>21.0</v>
+        <v>18.8</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>31.6263</v>
+        <v>26.4357</v>
       </c>
       <c r="H4" t="n">
         <v>6.0</v>
@@ -219,19 +222,19 @@
         <v>10.0</v>
       </c>
       <c r="C5" t="n">
-        <v>60.0</v>
+        <v>55.0</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>49.0</v>
+        <v>47.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>6.0</v>
+        <v>5.5</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>15.1217</v>
+        <v>14.6002</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
@@ -245,7 +248,7 @@
         <v>10.0</v>
       </c>
       <c r="C6" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
@@ -254,13 +257,13 @@
         <v>2.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>0.674949</v>
+        <v>0.707107</v>
       </c>
       <c r="H6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -271,19 +274,19 @@
         <v>10.0</v>
       </c>
       <c r="C7" t="n">
-        <v>276.0</v>
+        <v>290.0</v>
       </c>
       <c r="D7" t="n">
         <v>18.0</v>
       </c>
       <c r="E7" t="n">
-        <v>100.0</v>
+        <v>103.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>27.6</v>
+        <v>29.0</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>25.4698</v>
+        <v>26.1066</v>
       </c>
       <c r="H7" t="n">
         <v>18.0</v>
@@ -297,7 +300,7 @@
         <v>10.0</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
@@ -306,10 +309,10 @@
         <v>1.0</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="G8" t="n" s="2">
-        <v>0.421637</v>
+        <v>0.527046</v>
       </c>
       <c r="H8" t="n">
         <v>0.0</v>
@@ -323,21 +326,47 @@
         <v>10.0</v>
       </c>
       <c r="C9" t="n">
-        <v>70.0</v>
+        <v>13.0</v>
       </c>
       <c r="D9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F9" t="n" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="G9" t="n" s="2">
+        <v>0.948683</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="D10" t="n">
         <v>4.0</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>20.0</v>
       </c>
-      <c r="F9" t="n" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="G9" t="n" s="2">
-        <v>4.96655</v>
-      </c>
-      <c r="H9" t="n">
+      <c r="F10" t="n" s="2">
+        <v>7.1</v>
+      </c>
+      <c r="G10" t="n" s="2">
+        <v>4.8408</v>
+      </c>
+      <c r="H10" t="n">
         <v>4.0</v>
       </c>
     </row>
@@ -348,7 +377,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1.0" state="frozen" topLeftCell="B1" activePane="topRight"/>
@@ -393,22 +422,22 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C3" t="n">
-        <v>521.0</v>
+        <v>577.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>0.0119498</v>
+        <v>0.013832</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>0.108661</v>
+        <v>0.117</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -419,22 +448,22 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C4" t="n">
-        <v>184080.0</v>
+        <v>179094.0</v>
       </c>
       <c r="D4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E4" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>4.22212</v>
+        <v>4.29328</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>0.444059</v>
+        <v>0.469731</v>
       </c>
       <c r="H4" t="n">
         <v>5.0</v>
@@ -445,10 +474,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C5" t="n">
-        <v>11528.0</v>
+        <v>10937.0</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
@@ -457,10 +486,10 @@
         <v>5.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>0.26441</v>
+        <v>0.262184</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>0.443461</v>
+        <v>0.441297</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
@@ -471,22 +500,22 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C6" t="n">
-        <v>599.0</v>
+        <v>631.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>0.0137388</v>
+        <v>0.0151265</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>0.116406</v>
+        <v>0.122645</v>
       </c>
       <c r="H6" t="n">
         <v>0.0</v>
@@ -497,22 +526,22 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C7" t="n">
-        <v>257521.0</v>
+        <v>244636.0</v>
       </c>
       <c r="D7" t="n">
         <v>5.0</v>
       </c>
       <c r="E7" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>5.90658</v>
+        <v>5.86446</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>0.415879</v>
+        <v>0.431023</v>
       </c>
       <c r="H7" t="n">
         <v>6.0</v>
@@ -523,10 +552,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C8" t="n">
-        <v>268.0</v>
+        <v>271.0</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
@@ -535,10 +564,10 @@
         <v>1.0</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>0.00614693</v>
+        <v>0.00649646</v>
       </c>
       <c r="G8" t="n" s="2">
-        <v>0.0781619</v>
+        <v>0.0803394</v>
       </c>
       <c r="H8" t="n">
         <v>0.0</v>
@@ -549,233 +578,285 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>43599.0</v>
+        <v>41715.0</v>
       </c>
       <c r="C9" t="n">
-        <v>135118.0</v>
+        <v>16365.0</v>
       </c>
       <c r="D9" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="E9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F9" t="n" s="2">
+        <v>0.392305</v>
+      </c>
+      <c r="G9" t="n" s="2">
+        <v>0.490914</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="n">
+        <v>41715.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>135052.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E10" t="n">
         <v>12.0</v>
       </c>
-      <c r="F9" t="n" s="2">
-        <v>3.09911</v>
-      </c>
-      <c r="G9" t="n" s="2">
-        <v>0.373215</v>
-      </c>
-      <c r="H9" t="n">
+      <c r="F10" t="n" s="2">
+        <v>3.23749</v>
+      </c>
+      <c r="G10" t="n" s="2">
+        <v>0.46082</v>
+      </c>
+      <c r="H10" t="n">
         <v>3.0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="B12" t="n" s="1">
+    <row r="13">
+      <c r="A13" t="s" s="1">
+        <v>17</v>
+      </c>
+      <c r="B13" t="n" s="1">
         <v>10.0</v>
       </c>
-      <c r="C12" t="n" s="1">
+      <c r="C13" t="n" s="1">
         <v>100.0</v>
       </c>
-      <c r="D12" t="n" s="1">
+      <c r="D13" t="n" s="1">
         <v>1000.0</v>
       </c>
-      <c r="E12" t="n" s="1">
+      <c r="E13" t="n" s="1">
         <v>10000.0</v>
       </c>
-      <c r="F12" t="n" s="1">
+      <c r="F13" t="n" s="1">
         <v>20000.0</v>
       </c>
-      <c r="G12" t="n" s="1">
+      <c r="G13" t="n" s="1">
         <v>30000.0</v>
       </c>
-      <c r="H12" t="n" s="1">
+      <c r="H13" t="n" s="1">
         <v>40000.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="n" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C13" t="n" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="D13" t="n" s="2">
-        <v>0.014</v>
-      </c>
-      <c r="E13" t="n" s="2">
-        <v>0.013</v>
-      </c>
-      <c r="F13" t="n" s="2">
-        <v>0.01255</v>
-      </c>
-      <c r="G13" t="n" s="2">
-        <v>0.0120333</v>
-      </c>
-      <c r="H13" t="n" s="2">
-        <v>0.01195</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n" s="2">
-        <v>6.2</v>
+        <v>0.0</v>
       </c>
       <c r="C14" t="n" s="2">
-        <v>5.05</v>
+        <v>0.06</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>4.23</v>
+        <v>0.022</v>
       </c>
       <c r="E14" t="n" s="2">
-        <v>4.2055</v>
+        <v>0.0134</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>4.2329</v>
+        <v>0.01395</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>4.22363</v>
+        <v>0.0137</v>
       </c>
       <c r="H14" t="n" s="2">
-        <v>4.21545</v>
+        <v>0.0137</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="n" s="2">
-        <v>0.2</v>
+        <v>6.0</v>
       </c>
       <c r="C15" t="n" s="2">
-        <v>0.42</v>
+        <v>5.02</v>
       </c>
       <c r="D15" t="n" s="2">
-        <v>0.295</v>
+        <v>4.191</v>
       </c>
       <c r="E15" t="n" s="2">
-        <v>0.2694</v>
+        <v>4.2656</v>
       </c>
       <c r="F15" t="n" s="2">
-        <v>0.2672</v>
+        <v>4.2889</v>
       </c>
       <c r="G15" t="n" s="2">
-        <v>0.264</v>
+        <v>4.2926</v>
       </c>
       <c r="H15" t="n" s="2">
-        <v>0.264525</v>
+        <v>4.29318</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="n" s="2">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C16" t="n" s="2">
-        <v>0.07</v>
+        <v>0.35</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>0.031</v>
+        <v>0.296</v>
       </c>
       <c r="E16" t="n" s="2">
-        <v>0.0177</v>
+        <v>0.2666</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>0.0157</v>
+        <v>0.26455</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>0.0143333</v>
+        <v>0.2629</v>
       </c>
       <c r="H16" t="n" s="2">
-        <v>0.013825</v>
+        <v>0.262875</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" t="n" s="2">
-        <v>7.2</v>
+        <v>0.3</v>
       </c>
       <c r="C17" t="n" s="2">
-        <v>7.1</v>
+        <v>0.1</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>5.997</v>
+        <v>0.028</v>
       </c>
       <c r="E17" t="n" s="2">
-        <v>5.8877</v>
+        <v>0.0152</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>5.9214</v>
+        <v>0.0163</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>5.91257</v>
+        <v>0.0152667</v>
       </c>
       <c r="H17" t="n" s="2">
-        <v>5.89958</v>
+        <v>0.014975</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="n" s="2">
-        <v>0.3</v>
+        <v>7.9</v>
       </c>
       <c r="C18" t="n" s="2">
-        <v>0.39</v>
+        <v>6.92</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>0.058</v>
+        <v>5.839</v>
       </c>
       <c r="E18" t="n" s="2">
-        <v>0.0102</v>
+        <v>5.8406</v>
       </c>
       <c r="F18" t="n" s="2">
-        <v>0.00785</v>
+        <v>5.86255</v>
       </c>
       <c r="G18" t="n" s="2">
-        <v>0.0066</v>
+        <v>5.86243</v>
       </c>
       <c r="H18" t="n" s="2">
-        <v>0.006175</v>
+        <v>5.86408</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="n" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C19" t="n" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="D19" t="n" s="2">
+        <v>0.061</v>
+      </c>
+      <c r="E19" t="n" s="2">
+        <v>0.0108</v>
+      </c>
+      <c r="F19" t="n" s="2">
+        <v>0.00735</v>
+      </c>
+      <c r="G19" t="n" s="2">
+        <v>0.0069</v>
+      </c>
+      <c r="H19" t="n" s="2">
+        <v>0.006525</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="n" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="C19" t="n" s="2">
-        <v>3.91</v>
-      </c>
-      <c r="D19" t="n" s="2">
-        <v>3.19</v>
-      </c>
-      <c r="E19" t="n" s="2">
-        <v>3.0961</v>
-      </c>
-      <c r="F19" t="n" s="2">
-        <v>3.1112</v>
-      </c>
-      <c r="G19" t="n" s="2">
-        <v>3.1011</v>
-      </c>
-      <c r="H19" t="n" s="2">
-        <v>3.09528</v>
+      <c r="B20" t="n" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C20" t="n" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="D20" t="n" s="2">
+        <v>0.381</v>
+      </c>
+      <c r="E20" t="n" s="2">
+        <v>0.3894</v>
+      </c>
+      <c r="F20" t="n" s="2">
+        <v>0.39185</v>
+      </c>
+      <c r="G20" t="n" s="2">
+        <v>0.391733</v>
+      </c>
+      <c r="H20" t="n" s="2">
+        <v>0.3921</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="n" s="2">
+        <v>5.1</v>
+      </c>
+      <c r="C21" t="n" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="D21" t="n" s="2">
+        <v>3.241</v>
+      </c>
+      <c r="E21" t="n" s="2">
+        <v>3.2373</v>
+      </c>
+      <c r="F21" t="n" s="2">
+        <v>3.23745</v>
+      </c>
+      <c r="G21" t="n" s="2">
+        <v>3.23717</v>
+      </c>
+      <c r="H21" t="n" s="2">
+        <v>3.2374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>